<commit_message>
Change stationary battery LCI
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/RTE_scenarios/inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/RTE_scenarios/inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABFED1-4056-3742-BB91-689DDADCEBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428A29F3-888A-5543-B8E8-5CAC9CF2C18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28340" windowHeight="26420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28340" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="105">
   <si>
     <t>Database</t>
   </si>
@@ -276,13 +276,94 @@
   </si>
   <si>
     <t>hydrogen production, gaseous, 30 bar, from PEM electrolysis, from grid electricity, domestic, FE2050</t>
+  </si>
+  <si>
+    <t>electricity supply, high voltage, from vanadium-redox flow battery system</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>The power capacity for this application is 1MW and the net storage capacity 6 MWh. The net capacity considers the internal inefficiencies of the batteries and the min SoC, requiring a certain oversizing of the batteries. For providing net 6 MWh, a nominal capacity of 8.3 MWh is required for the VRFB with the assumed operation parameters. The assumed lifetime of the stack is 10 years. The lifetimeof the system is 20 years or 8176 cycle-lifes (49,000 MWh).</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Life Cycle Assessment of a Vanadium Redox Flow Battery, Selina Weber, Jens F. Peters, Manuel Baumann, and Marcel Weil, Environ. Sci. Technol. 2018, 52, 10864−10873, DOI: 10.1021/acs.est.8b02073</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>Electricity input plus losses</t>
+  </si>
+  <si>
+    <t>vanadium-redox flow battery system assembly, 8.3 megawatt hour</t>
+  </si>
+  <si>
+    <t>vanadium-redox flow battery system</t>
+  </si>
+  <si>
+    <t>Infrastructure requirements 1/49000 MWh</t>
+  </si>
+  <si>
+    <t>vanadium-redox flow battery stack assembly</t>
+  </si>
+  <si>
+    <t>vanadium-redox flow battery stack</t>
+  </si>
+  <si>
+    <t>Replacement stack</t>
+  </si>
+  <si>
+    <t>treatment of stack, for VRFB system</t>
+  </si>
+  <si>
+    <t>used stack, for VRFB system</t>
+  </si>
+  <si>
+    <t>EoL of both stack</t>
+  </si>
+  <si>
+    <t>treatment of electrolyte tank, for VRFB system</t>
+  </si>
+  <si>
+    <t>used electrolyte tank, for VRFB system</t>
+  </si>
+  <si>
+    <t>Electrolyte tank EoL</t>
+  </si>
+  <si>
+    <t>treatment of electrolyte solution, for VRFB system</t>
+  </si>
+  <si>
+    <t>used electrolyte solution, for VRFB system</t>
+  </si>
+  <si>
+    <t>Electrolyte EoL</t>
+  </si>
+  <si>
+    <t>treatment of periphericals, for VRFB system</t>
+  </si>
+  <si>
+    <t>used periphericals, for VRFB system</t>
+  </si>
+  <si>
+    <t>Peripherals EoL</t>
+  </si>
+  <si>
+    <t>market for electricity, high voltage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +437,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -395,7 +484,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -446,6 +535,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
@@ -730,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T87"/>
+  <dimension ref="A1:T107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2237,7 +2328,7 @@
       <c r="G80" s="16"/>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2263,7 +2354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -2284,7 +2375,7 @@
       </c>
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>38</v>
       </c>
@@ -2305,7 +2396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -2325,7 +2416,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -2345,7 +2436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -2365,7 +2456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -2384,6 +2475,345 @@
       <c r="F87" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="I89"/>
+      <c r="M89" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90"/>
+      <c r="M90" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>81</v>
+      </c>
+      <c r="I91"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="I92"/>
+      <c r="M92" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
+      <c r="I93"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+      <c r="I94"/>
+      <c r="M94" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>84</v>
+      </c>
+      <c r="I95"/>
+      <c r="M95" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>19</v>
+      </c>
+      <c r="I96"/>
+      <c r="M96" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97"/>
+      <c r="I97"/>
+      <c r="M97" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H98" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I98" s="40"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" t="str">
+        <f>B89</f>
+        <v>electricity supply, high voltage, from vanadium-redox flow battery system</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" t="str">
+        <f>B96</f>
+        <v>kilowatt hour</v>
+      </c>
+      <c r="F99" t="s">
+        <v>18</v>
+      </c>
+      <c r="G99" t="str">
+        <f>B94</f>
+        <v>electricity, high voltage</v>
+      </c>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="8"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100">
+        <v>1.33</v>
+      </c>
+      <c r="C100" t="s">
+        <v>30</v>
+      </c>
+      <c r="D100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
+        <v>32</v>
+      </c>
+      <c r="H100" t="s">
+        <v>85</v>
+      </c>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="8"/>
+      <c r="N100" s="8"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" s="41">
+        <f>1/(49000000)</f>
+        <v>2.0408163265306123E-8</v>
+      </c>
+      <c r="C101" t="s">
+        <v>52</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="F101" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" t="s">
+        <v>87</v>
+      </c>
+      <c r="H101" t="s">
+        <v>88</v>
+      </c>
+      <c r="I101"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>89</v>
+      </c>
+      <c r="B102" s="41">
+        <f>1/(49000000)</f>
+        <v>2.0408163265306123E-8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>52</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="F102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" t="s">
+        <v>90</v>
+      </c>
+      <c r="H102" t="s">
+        <v>91</v>
+      </c>
+      <c r="I102"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>92</v>
+      </c>
+      <c r="B103" s="41">
+        <f>-0.41/1000</f>
+        <v>-4.0999999999999999E-4</v>
+      </c>
+      <c r="C103" t="s">
+        <v>52</v>
+      </c>
+      <c r="D103" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" t="s">
+        <v>93</v>
+      </c>
+      <c r="H103" t="s">
+        <v>94</v>
+      </c>
+      <c r="I103"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104">
+        <f>-0.66/1000</f>
+        <v>-6.6E-4</v>
+      </c>
+      <c r="C104" t="s">
+        <v>52</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
+        <v>96</v>
+      </c>
+      <c r="H104" t="s">
+        <v>97</v>
+      </c>
+      <c r="I104"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B105">
+        <f>-5.55/1000</f>
+        <v>-5.5500000000000002E-3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>52</v>
+      </c>
+      <c r="D105" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" t="s">
+        <v>99</v>
+      </c>
+      <c r="H105" t="s">
+        <v>100</v>
+      </c>
+      <c r="I105"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106">
+        <f>-0.1/1000</f>
+        <v>-1E-4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>52</v>
+      </c>
+      <c r="D106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" t="s">
+        <v>102</v>
+      </c>
+      <c r="H106" t="s">
+        <v>103</v>
+      </c>
+      <c r="I106"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B107"/>
+      <c r="I107"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated electricity RER to FR
Activity updated: hydrogen production, gaseous, 30 bar, from PEM electrolysis, from grid electricity, domestic, FE2050

electricity RER to FR
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/RTE_scenarios/inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsteinbach\Documents\GitHub\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64507A8-3861-BC47-98A2-BEB02A9347E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB8B134-176F-4FFD-A9A4-318DC36D1F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28340" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,25 +823,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="99.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="55.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="99.1796875" style="3" customWidth="1"/>
     <col min="10" max="10" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="I2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -877,7 +877,7 @@
       <c r="I3" s="7"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="I4" s="11"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="I5" s="11"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="I6" s="11"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -941,7 +941,7 @@
       <c r="I7" s="11"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -957,7 +957,7 @@
       <c r="I8" s="11"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -973,7 +973,7 @@
       <c r="I9" s="17"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
@@ -987,7 +987,7 @@
       <c r="I10" s="18"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="H12" s="18"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1062,19 +1062,19 @@
       <c r="G13" s="13"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="19"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="19"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="I16" s="11"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="I17" s="11"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="6" t="s">
         <v>11</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="I18" s="11"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="I19" s="11"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="I20" s="11"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="I21" s="17"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="16" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="I22" s="18"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="19" t="s">
         <v>36</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="H24" s="18"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="6" t="s">
         <v>58</v>
       </c>
@@ -1311,13 +1311,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="19"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="I29" s="11"/>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="6" t="s">
         <v>3</v>
       </c>
@@ -1349,7 +1349,7 @@
       <c r="I30" s="11"/>
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="6" t="s">
         <v>11</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="I31" s="11"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="I32" s="11"/>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20">
       <c r="A33" s="6" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="I33" s="11"/>
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20">
       <c r="A34" s="6" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="I34" s="17"/>
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20">
       <c r="A35" s="16" t="s">
         <v>7</v>
       </c>
@@ -1427,7 +1427,7 @@
       <c r="I35" s="18"/>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20">
       <c r="A37" s="19" t="s">
         <v>31</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="H37" s="18"/>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20">
       <c r="A38" s="19" t="s">
         <v>33</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="H38" s="18"/>
       <c r="K38" s="8"/>
     </row>
-    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="15.5">
       <c r="A39" s="32" t="s">
         <v>78</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="I39" s="18"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="9"/>
@@ -1539,7 +1539,7 @@
       <c r="I40" s="11"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A41" s="24" t="s">
         <v>1</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="O41" s="28"/>
       <c r="P41" s="28"/>
     </row>
-    <row r="42" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A42" s="29" t="s">
         <v>3</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="O42" s="28"/>
       <c r="P42" s="28"/>
     </row>
-    <row r="43" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A43" s="29" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="O43" s="28"/>
       <c r="P43" s="28"/>
     </row>
-    <row r="44" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A44" s="29" t="s">
         <v>4</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="O44" s="28"/>
       <c r="P44" s="28"/>
     </row>
-    <row r="45" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A45" s="29" t="s">
         <v>2</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="O45" s="28"/>
       <c r="P45" s="28"/>
     </row>
-    <row r="46" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A46" s="29" t="s">
         <v>6</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="O46" s="28"/>
       <c r="P46" s="28"/>
     </row>
-    <row r="47" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A47" s="33" t="s">
         <v>7</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="O47" s="28"/>
       <c r="P47" s="28"/>
     </row>
-    <row r="48" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A48" s="33" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="S48" s="33"/>
       <c r="T48" s="34"/>
     </row>
-    <row r="49" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A49" s="32" t="s">
         <v>78</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="P49" s="28"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A50" s="32" t="s">
         <v>76</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="Q50"/>
       <c r="R50"/>
     </row>
-    <row r="51" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A51" s="32" t="s">
         <v>77</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="Q51"/>
       <c r="R51"/>
     </row>
-    <row r="52" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A52" s="32" t="s">
         <v>67</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="Q52"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A53" s="32" t="s">
         <v>70</v>
       </c>
@@ -1849,7 +1849,7 @@
       <c r="Q53"/>
       <c r="R53"/>
     </row>
-    <row r="54" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A54" s="29" t="s">
         <v>53</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>54</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D54" s="27" t="s">
         <v>19</v>
@@ -1882,7 +1882,7 @@
       <c r="Q54"/>
       <c r="R54"/>
     </row>
-    <row r="55" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A55" s="29" t="s">
         <v>21</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="Q55"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A56" s="38" t="s">
         <v>24</v>
       </c>
@@ -1943,7 +1943,7 @@
       <c r="Q56" s="36"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A57" s="38" t="s">
         <v>75</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="Q57" s="36"/>
       <c r="R57"/>
     </row>
-    <row r="58" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
       <c r="M58" s="28"/>
@@ -1981,7 +1981,7 @@
       <c r="O58" s="28"/>
       <c r="P58" s="28"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20">
       <c r="A59" s="4" t="s">
         <v>1</v>
       </c>
@@ -1997,7 +1997,7 @@
       <c r="J59" s="21"/>
       <c r="K59" s="22"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20">
       <c r="A60" s="6" t="s">
         <v>3</v>
       </c>
@@ -2013,7 +2013,7 @@
       <c r="J60" s="13"/>
       <c r="K60" s="22"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20">
       <c r="A61" s="6" t="s">
         <v>11</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="H61" s="9"/>
       <c r="K61" s="22"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:20" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="16.25" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>2</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20">
       <c r="A64" s="6" t="s">
         <v>6</v>
       </c>
@@ -2070,7 +2070,7 @@
       <c r="G64" s="9"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" s="16" t="s">
         <v>7</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="G65" s="16"/>
       <c r="H65" s="13"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" s="4" t="s">
         <v>1</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="J74" s="21"/>
       <c r="K74" s="22"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" s="6" t="s">
         <v>3</v>
       </c>
@@ -2259,7 +2259,7 @@
       <c r="J75" s="13"/>
       <c r="K75" s="22"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" s="6" t="s">
         <v>11</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="H76" s="9"/>
       <c r="K76" s="22"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" s="6" t="s">
         <v>4</v>
       </c>
@@ -2288,7 +2288,7 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:11" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="16.25" customHeight="1">
       <c r="A78" s="6" t="s">
         <v>2</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11">
       <c r="A79" s="6" t="s">
         <v>6</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="G79" s="9"/>
       <c r="H79" s="16"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80" s="16" t="s">
         <v>7</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="G80" s="16"/>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>38</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" ht="15.5">
       <c r="A89" s="34" t="s">
         <v>1</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="I91"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>82</v>
       </c>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="15.5">
       <c r="A97" s="34" t="s">
         <v>7</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="15.5">
       <c r="A98" s="34" t="s">
         <v>8</v>
       </c>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="I98" s="40"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14">
       <c r="A99" t="str">
         <f>B89</f>
         <v>electricity supply, high voltage, from vanadium-redox flow battery system</v>
@@ -2632,7 +2632,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="8"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -2661,7 +2661,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="8"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14">
       <c r="A101" t="s">
         <v>86</v>
       </c>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14">
       <c r="A103" t="s">
         <v>92</v>
       </c>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14">
       <c r="A104" t="s">
         <v>95</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="I104"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="I105"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14">
       <c r="B107"/>
       <c r="I107"/>
     </row>

</xml_diff>

<commit_message>
removed "group" from activity name
When switching from RER to FR the activity name should also change from market group for electricity to market for electricity
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsteinbach\Documents\GitHub\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB8B134-176F-4FFD-A9A4-318DC36D1F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0594B77C-9845-4C77-80E6-B551673DAACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="104">
   <si>
     <t>Database</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>RER</t>
-  </si>
-  <si>
-    <t>market group for electricity, low voltage</t>
   </si>
   <si>
     <t>1 kWh of electricity discharged from a BEV. Accounts for charge and discharge losses: 15% and 12%, in 2020, respectively.</t>
@@ -823,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -914,7 +911,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1111,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1258,7 +1255,7 @@
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1283,12 +1280,12 @@
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="19">
         <f>1/(2500*80%*19.5)</f>
@@ -1304,11 +1301,11 @@
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1505,7 +1502,7 @@
     </row>
     <row r="39" spans="1:20" ht="15.5">
       <c r="A39" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="19">
         <f>3.6/0.5/120</f>
@@ -1521,7 +1518,7 @@
         <v>12</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="18"/>
@@ -1544,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="26"/>
       <c r="K41" s="28"/>
@@ -1573,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K43" s="28"/>
       <c r="L43" s="28"/>
@@ -1587,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K44" s="28"/>
       <c r="L44" s="28"/>
@@ -1687,7 +1684,7 @@
     </row>
     <row r="49" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A49" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="32">
         <v>1</v>
@@ -1705,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="50" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A50" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="27">
         <f>(1/2963200)*4</f>
@@ -1735,10 +1732,10 @@
         <v>12</v>
       </c>
       <c r="G50" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" s="27" t="s">
         <v>63</v>
-      </c>
-      <c r="H50" s="27" t="s">
-        <v>64</v>
       </c>
       <c r="J50"/>
       <c r="K50" s="36"/>
@@ -1752,7 +1749,7 @@
     </row>
     <row r="51" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A51" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="27">
         <f>1/2963200</f>
@@ -1768,10 +1765,10 @@
         <v>12</v>
       </c>
       <c r="G51" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" s="27" t="s">
         <v>65</v>
-      </c>
-      <c r="H51" s="27" t="s">
-        <v>66</v>
       </c>
       <c r="J51"/>
       <c r="K51" s="36"/>
@@ -1785,7 +1782,7 @@
     </row>
     <row r="52" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A52" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="27">
         <f>B50*-1</f>
@@ -1801,10 +1798,10 @@
         <v>12</v>
       </c>
       <c r="G52" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H52" s="27" t="s">
         <v>68</v>
-      </c>
-      <c r="H52" s="27" t="s">
-        <v>69</v>
       </c>
       <c r="J52"/>
       <c r="K52" s="36"/>
@@ -1818,7 +1815,7 @@
     </row>
     <row r="53" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A53" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" s="27">
         <f>-1*B51</f>
@@ -1834,10 +1831,10 @@
         <v>12</v>
       </c>
       <c r="G53" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H53" s="27" t="s">
         <v>71</v>
-      </c>
-      <c r="H53" s="27" t="s">
-        <v>72</v>
       </c>
       <c r="J53"/>
       <c r="K53" s="36"/>
@@ -1851,7 +1848,7 @@
     </row>
     <row r="54" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A54" s="29" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B54" s="32">
         <v>54</v>
@@ -1870,7 +1867,7 @@
         <v>20</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J54"/>
       <c r="K54" s="36"/>
@@ -1902,7 +1899,7 @@
         <v>23</v>
       </c>
       <c r="H55" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J55"/>
       <c r="K55" s="36"/>
@@ -1945,7 +1942,7 @@
     </row>
     <row r="57" spans="1:20" s="27" customFormat="1" ht="15.5">
       <c r="A57" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" s="31">
         <f>(0.09*1000*20)/2963200</f>
@@ -2481,11 +2478,11 @@
         <v>1</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I89"/>
       <c r="M89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -2497,7 +2494,7 @@
       </c>
       <c r="I90"/>
       <c r="M90" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:13">
@@ -2505,7 +2502,7 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I91"/>
     </row>
@@ -2518,15 +2515,15 @@
       </c>
       <c r="I92"/>
       <c r="M92" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" t="s">
         <v>82</v>
-      </c>
-      <c r="B93" t="s">
-        <v>83</v>
       </c>
       <c r="I93"/>
     </row>
@@ -2539,7 +2536,7 @@
       </c>
       <c r="I94"/>
       <c r="M94" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -2547,11 +2544,11 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I95"/>
       <c r="M95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -2563,7 +2560,7 @@
       </c>
       <c r="I96"/>
       <c r="M96" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15.5">
@@ -2573,7 +2570,7 @@
       <c r="B97"/>
       <c r="I97"/>
       <c r="M97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="15.5">
@@ -2634,7 +2631,7 @@
     </row>
     <row r="100" spans="1:14">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>1.33</v>
@@ -2652,7 +2649,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
@@ -2663,7 +2660,7 @@
     </row>
     <row r="101" spans="1:14">
       <c r="A101" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B101" s="41">
         <f>1/(49000000)</f>
@@ -2679,16 +2676,16 @@
         <v>12</v>
       </c>
       <c r="G101" t="s">
+        <v>86</v>
+      </c>
+      <c r="H101" t="s">
         <v>87</v>
-      </c>
-      <c r="H101" t="s">
-        <v>88</v>
       </c>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B102" s="41">
         <f>1/(49000000)</f>
@@ -2704,16 +2701,16 @@
         <v>12</v>
       </c>
       <c r="G102" t="s">
+        <v>89</v>
+      </c>
+      <c r="H102" t="s">
         <v>90</v>
-      </c>
-      <c r="H102" t="s">
-        <v>91</v>
       </c>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B103" s="41">
         <f>-0.41/1000</f>
@@ -2729,16 +2726,16 @@
         <v>12</v>
       </c>
       <c r="G103" t="s">
+        <v>92</v>
+      </c>
+      <c r="H103" t="s">
         <v>93</v>
-      </c>
-      <c r="H103" t="s">
-        <v>94</v>
       </c>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B104">
         <f>-0.66/1000</f>
@@ -2754,16 +2751,16 @@
         <v>12</v>
       </c>
       <c r="G104" t="s">
+        <v>95</v>
+      </c>
+      <c r="H104" t="s">
         <v>96</v>
-      </c>
-      <c r="H104" t="s">
-        <v>97</v>
       </c>
       <c r="I104"/>
     </row>
     <row r="105" spans="1:14">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105">
         <f>-5.55/1000</f>
@@ -2779,16 +2776,16 @@
         <v>12</v>
       </c>
       <c r="G105" t="s">
+        <v>98</v>
+      </c>
+      <c r="H105" t="s">
         <v>99</v>
-      </c>
-      <c r="H105" t="s">
-        <v>100</v>
       </c>
       <c r="I105"/>
     </row>
     <row r="106" spans="1:14">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106">
         <f>-0.1/1000</f>
@@ -2804,10 +2801,10 @@
         <v>12</v>
       </c>
       <c r="G106" t="s">
+        <v>101</v>
+      </c>
+      <c r="H106" t="s">
         <v>102</v>
-      </c>
-      <c r="H106" t="s">
-        <v>103</v>
       </c>
       <c r="I106"/>
     </row>

</xml_diff>

<commit_message>
Correct electricity input in FR electrolysis dataset.
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsteinbach\Documents\GitHub\RTE_scenarios\inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/RTE_scenarios/inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0594B77C-9845-4C77-80E6-B551673DAACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618BBD32-09E5-BB4A-8CF7-C0E80DFC0C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28340" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="104">
   <si>
     <t>Database</t>
   </si>
@@ -360,7 +360,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,25 +820,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.6328125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="99.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="99.1640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -846,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -862,7 +862,7 @@
       <c r="I2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -874,7 +874,7 @@
       <c r="I3" s="7"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="I4" s="11"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="I5" s="11"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -922,7 +922,7 @@
       <c r="I6" s="11"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="I7" s="11"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -954,7 +954,7 @@
       <c r="I8" s="11"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="I9" s="17"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="I10" s="18"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="H12" s="18"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1059,19 +1059,19 @@
       <c r="G13" s="13"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="I16" s="11"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="I17" s="11"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>11</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="I18" s="11"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="I19" s="11"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="I20" s="11"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="I21" s="17"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="I22" s="18"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1209,9 +1209,10 @@
       <c r="J23" s="1"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="19" t="s">
-        <v>36</v>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="str">
+        <f>B16</f>
+        <v>electricity production, from stationary battery, FE2050</v>
       </c>
       <c r="B24" s="19">
         <v>1</v>
@@ -1233,7 +1234,7 @@
       <c r="H24" s="18"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>57</v>
       </c>
@@ -1308,13 +1309,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
@@ -1330,7 +1331,7 @@
       <c r="I29" s="11"/>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>3</v>
       </c>
@@ -1346,7 +1347,7 @@
       <c r="I30" s="11"/>
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>11</v>
       </c>
@@ -1362,7 +1363,7 @@
       <c r="I31" s="11"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -1378,7 +1379,7 @@
       <c r="I32" s="11"/>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>2</v>
       </c>
@@ -1394,7 +1395,7 @@
       <c r="I33" s="11"/>
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1411,7 @@
       <c r="I34" s="17"/>
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>7</v>
       </c>
@@ -1424,7 +1425,7 @@
       <c r="I35" s="18"/>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1452,7 +1453,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1477,7 @@
       <c r="H37" s="18"/>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>33</v>
       </c>
@@ -1500,7 +1501,7 @@
       <c r="H38" s="18"/>
       <c r="K38" s="8"/>
     </row>
-    <row r="39" spans="1:20" ht="15.5">
+    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>77</v>
       </c>
@@ -1524,7 +1525,7 @@
       <c r="I39" s="18"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="9"/>
@@ -1536,7 +1537,7 @@
       <c r="I40" s="11"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="41" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
         <v>1</v>
       </c>
@@ -1551,7 +1552,7 @@
       <c r="O41" s="28"/>
       <c r="P41" s="28"/>
     </row>
-    <row r="42" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="42" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="s">
         <v>3</v>
       </c>
@@ -1565,7 +1566,7 @@
       <c r="O42" s="28"/>
       <c r="P42" s="28"/>
     </row>
-    <row r="43" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="43" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="29" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1580,7 @@
       <c r="O43" s="28"/>
       <c r="P43" s="28"/>
     </row>
-    <row r="44" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="44" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="29" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1594,7 @@
       <c r="O44" s="28"/>
       <c r="P44" s="28"/>
     </row>
-    <row r="45" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="45" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="29" t="s">
         <v>2</v>
       </c>
@@ -1607,7 +1608,7 @@
       <c r="O45" s="28"/>
       <c r="P45" s="28"/>
     </row>
-    <row r="46" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="46" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="29" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1625,7 @@
       <c r="O46" s="28"/>
       <c r="P46" s="28"/>
     </row>
-    <row r="47" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="47" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="33" t="s">
         <v>7</v>
       </c>
@@ -1644,7 +1645,7 @@
       <c r="O47" s="28"/>
       <c r="P47" s="28"/>
     </row>
-    <row r="48" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="48" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="33" t="s">
         <v>8</v>
       </c>
@@ -1682,7 +1683,7 @@
       <c r="S48" s="33"/>
       <c r="T48" s="34"/>
     </row>
-    <row r="49" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="49" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
         <v>77</v>
       </c>
@@ -1714,7 +1715,7 @@
       <c r="P49" s="28"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="50" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>75</v>
       </c>
@@ -1747,7 +1748,7 @@
       <c r="Q50"/>
       <c r="R50"/>
     </row>
-    <row r="51" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="51" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>76</v>
       </c>
@@ -1780,7 +1781,7 @@
       <c r="Q51"/>
       <c r="R51"/>
     </row>
-    <row r="52" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="52" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>66</v>
       </c>
@@ -1813,7 +1814,7 @@
       <c r="Q52"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="53" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>69</v>
       </c>
@@ -1846,7 +1847,7 @@
       <c r="Q53"/>
       <c r="R53"/>
     </row>
-    <row r="54" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="54" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="29" t="s">
         <v>28</v>
       </c>
@@ -1879,7 +1880,7 @@
       <c r="Q54"/>
       <c r="R54"/>
     </row>
-    <row r="55" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="55" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="29" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1912,7 @@
       <c r="Q55"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="56" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="38" t="s">
         <v>24</v>
       </c>
@@ -1940,7 +1941,7 @@
       <c r="Q56" s="36"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="57" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="s">
         <v>74</v>
       </c>
@@ -1970,7 +1971,7 @@
       <c r="Q57" s="36"/>
       <c r="R57"/>
     </row>
-    <row r="58" spans="1:20" s="27" customFormat="1" ht="15.5">
+    <row r="58" spans="1:20" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
       <c r="M58" s="28"/>
@@ -1978,7 +1979,7 @@
       <c r="O58" s="28"/>
       <c r="P58" s="28"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +1995,7 @@
       <c r="J59" s="21"/>
       <c r="K59" s="22"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>3</v>
       </c>
@@ -2010,7 +2011,7 @@
       <c r="J60" s="13"/>
       <c r="K60" s="22"/>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>11</v>
       </c>
@@ -2025,7 +2026,7 @@
       <c r="H61" s="9"/>
       <c r="K61" s="22"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2040,7 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:20" ht="16.25" customHeight="1">
+    <row r="63" spans="1:20" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>2</v>
       </c>
@@ -2053,7 +2054,7 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>6</v>
       </c>
@@ -2067,7 +2068,7 @@
       <c r="G64" s="9"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
         <v>7</v>
       </c>
@@ -2079,7 +2080,7 @@
       <c r="G65" s="16"/>
       <c r="H65" s="13"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -2126,7 +2127,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -2147,7 +2148,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>1</v>
       </c>
@@ -2240,7 +2241,7 @@
       <c r="J74" s="21"/>
       <c r="K74" s="22"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>3</v>
       </c>
@@ -2256,7 +2257,7 @@
       <c r="J75" s="13"/>
       <c r="K75" s="22"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>11</v>
       </c>
@@ -2271,7 +2272,7 @@
       <c r="H76" s="9"/>
       <c r="K76" s="22"/>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>4</v>
       </c>
@@ -2285,7 +2286,7 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:11" ht="16.25" customHeight="1">
+    <row r="78" spans="1:11" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>2</v>
       </c>
@@ -2299,7 +2300,7 @@
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2314,7 @@
       <c r="G79" s="9"/>
       <c r="H79" s="16"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
         <v>7</v>
       </c>
@@ -2325,7 +2326,7 @@
       <c r="G80" s="16"/>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -2372,7 +2373,7 @@
       </c>
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>38</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="15.5">
+    <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="34" t="s">
         <v>1</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -2506,7 +2507,7 @@
       </c>
       <c r="I91"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>81</v>
       </c>
@@ -2527,7 +2528,7 @@
       </c>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2563,7 +2564,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="15.5">
+    <row r="97" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="34" t="s">
         <v>7</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="15.5">
+    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="34" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2601,7 @@
       </c>
       <c r="I98" s="40"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>B89</f>
         <v>electricity supply, high voltage, from vanadium-redox flow battery system</v>
@@ -2629,7 +2630,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="8"/>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2658,7 +2659,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="8"/>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -2683,7 +2684,7 @@
       </c>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -2708,7 +2709,7 @@
       </c>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -2733,7 +2734,7 @@
       </c>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>94</v>
       </c>
@@ -2758,7 +2759,7 @@
       </c>
       <c r="I104"/>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -2783,7 +2784,7 @@
       </c>
       <c r="I105"/>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>100</v>
       </c>
@@ -2808,7 +2809,7 @@
       </c>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B107"/>
       <c r="I107"/>
     </row>

</xml_diff>

<commit_message>
change coke activities to be compatible with ei310
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschlesinger\0.Joanna\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2D8C52-9E79-4761-9EB3-545791DA9922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F494C068-2186-4BD4-A197-3C8B1E7A1073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,9 +136,6 @@
     <t>electricity production, from stationary battery, FE2050</t>
   </si>
   <si>
-    <t>coking</t>
-  </si>
-  <si>
     <t>coal gas</t>
   </si>
   <si>
@@ -441,6 +438,9 @@
   </si>
   <si>
     <t>air::non-urban air or from high stacks</t>
+  </si>
+  <si>
+    <t>coke production</t>
   </si>
 </sst>
 </file>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1021,7 +1021,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="9"/>
@@ -1212,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="19">
         <v>1</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="19">
         <v>4.0404040404040398E-13</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1354,18 +1354,18 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" s="19">
         <v>7.5599999999999996E-6</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -1374,12 +1374,12 @@
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="19">
         <v>-7.5599999999999996E-6</v>
@@ -1394,12 +1394,12 @@
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="19">
         <v>1.25125</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B28" s="19">
         <v>7.7000000000000001E-8</v>
@@ -1431,12 +1431,12 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="19">
         <v>1.4E-5</v>
@@ -1448,18 +1448,18 @@
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" s="19">
         <v>2.49876858810916E-4</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1470,24 +1470,24 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31" s="19">
         <v>1.1580501231411899</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="19">
         <v>3.4499999999999999E-3</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="19">
         <v>2.3E-5</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1521,13 +1521,13 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="19">
         <v>2.2999999999999999E-7</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -1538,13 +1538,13 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="19">
         <v>2.2770000000000001E-5</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1555,36 +1555,36 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="19">
         <v>0.15</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="19">
         <v>1.1583000000000001</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="9"/>
@@ -1630,7 +1630,7 @@
         <v>11</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="19">
         <v>1</v>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" s="19">
         <v>1.3888999999999999E-11</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1772,7 +1772,7 @@
         <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G48" s="13"/>
       <c r="H48" s="18"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="19">
         <v>4.9730000000000003E-2</v>
@@ -1795,7 +1795,7 @@
         <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="18"/>
@@ -1803,19 +1803,19 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B50" s="19">
         <v>4.4479999999999899E-4</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="18"/>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" s="19">
         <v>1.5428571428571401E-4</v>
@@ -1835,7 +1835,7 @@
         <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="18"/>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B52" s="19">
         <v>2.47445129042634E-4</v>
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="9"/>
@@ -1904,7 +1904,7 @@
         <v>11</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -1920,7 +1920,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="19">
         <v>1</v>
@@ -2023,7 +2023,7 @@
         <v>18</v>
       </c>
       <c r="F62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="18"/>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B63">
         <v>1.0093999999999901</v>
@@ -2046,7 +2046,7 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G63" s="13"/>
       <c r="H63" s="18"/>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B64">
         <v>1.0093999999999901</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -2069,7 +2069,7 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="65" spans="1:20">
       <c r="A65" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" s="19">
         <v>0.88</v>
@@ -2092,7 +2092,7 @@
         <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="18"/>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="66" spans="1:20">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B66">
         <v>9.3999999999998494E-3</v>
@@ -2130,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="35"/>
@@ -2172,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="B70" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" s="35"/>
       <c r="D70" s="35"/>
@@ -2193,7 +2193,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C71" s="35"/>
       <c r="D71" s="35"/>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="76" spans="1:20" s="25" customFormat="1" ht="15.5">
       <c r="A76" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" s="44">
         <v>1</v>
@@ -2330,7 +2330,7 @@
         <v>18</v>
       </c>
       <c r="G76" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H76" s="40"/>
       <c r="I76" s="40"/>
@@ -2344,14 +2344,14 @@
     </row>
     <row r="77" spans="1:20" s="25" customFormat="1" ht="15.5">
       <c r="A77" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B77" s="35">
         <f>(1/2963200)*4</f>
         <v>1.3498920086393089E-6</v>
       </c>
       <c r="C77" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D77" s="35" t="s">
         <v>6</v>
@@ -2361,10 +2361,10 @@
         <v>12</v>
       </c>
       <c r="G77" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="H77" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="H77" s="35" t="s">
-        <v>58</v>
       </c>
       <c r="I77" s="35"/>
       <c r="J77"/>
@@ -2379,14 +2379,14 @@
     </row>
     <row r="78" spans="1:20" s="25" customFormat="1" ht="15.5">
       <c r="A78" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="35">
         <f>1/2963200</f>
         <v>3.3747300215982723E-7</v>
       </c>
       <c r="C78" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D78" s="35" t="s">
         <v>6</v>
@@ -2396,10 +2396,10 @@
         <v>12</v>
       </c>
       <c r="G78" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H78" s="35" t="s">
         <v>59</v>
-      </c>
-      <c r="H78" s="35" t="s">
-        <v>60</v>
       </c>
       <c r="I78" s="35"/>
       <c r="J78"/>
@@ -2414,14 +2414,14 @@
     </row>
     <row r="79" spans="1:20" s="25" customFormat="1" ht="15.5">
       <c r="A79" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B79" s="35">
         <f>B77*-1</f>
         <v>-1.3498920086393089E-6</v>
       </c>
       <c r="C79" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D79" s="35" t="s">
         <v>6</v>
@@ -2431,10 +2431,10 @@
         <v>12</v>
       </c>
       <c r="G79" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="H79" s="35" t="s">
         <v>62</v>
-      </c>
-      <c r="H79" s="35" t="s">
-        <v>63</v>
       </c>
       <c r="I79" s="35"/>
       <c r="J79"/>
@@ -2449,14 +2449,14 @@
     </row>
     <row r="80" spans="1:20" s="25" customFormat="1" ht="15.5">
       <c r="A80" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80" s="35">
         <f>-1*B78</f>
         <v>-3.3747300215982723E-7</v>
       </c>
       <c r="C80" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D80" s="35" t="s">
         <v>6</v>
@@ -2466,10 +2466,10 @@
         <v>12</v>
       </c>
       <c r="G80" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="35" t="s">
         <v>65</v>
-      </c>
-      <c r="H80" s="35" t="s">
-        <v>66</v>
       </c>
       <c r="I80" s="35"/>
       <c r="J80"/>
@@ -2503,7 +2503,7 @@
         <v>20</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I81" s="35"/>
       <c r="J81"/>
@@ -2537,7 +2537,7 @@
         <v>23</v>
       </c>
       <c r="H82" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I82" s="35"/>
       <c r="J82"/>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="84" spans="1:18" s="25" customFormat="1" ht="15.5">
       <c r="A84" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" s="43">
         <f>(0.09*1000*20)/2963200</f>
@@ -2644,11 +2644,11 @@
         <v>1</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I87"/>
       <c r="M87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:18">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="I88"/>
       <c r="M88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:18">
@@ -2668,7 +2668,7 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I89"/>
     </row>
@@ -2681,15 +2681,15 @@
       </c>
       <c r="I90"/>
       <c r="M90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:18">
       <c r="A91" t="s">
+        <v>73</v>
+      </c>
+      <c r="B91" t="s">
         <v>74</v>
-      </c>
-      <c r="B91" t="s">
-        <v>75</v>
       </c>
       <c r="I91"/>
     </row>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="I92"/>
       <c r="M92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:18">
@@ -2710,11 +2710,11 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I93"/>
       <c r="M93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:18">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="I94"/>
       <c r="M94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="15.5">
@@ -2736,7 +2736,7 @@
       <c r="B95"/>
       <c r="I95"/>
       <c r="M95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="15.5">
@@ -2797,7 +2797,7 @@
     </row>
     <row r="98" spans="1:14">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98">
         <v>1.33</v>
@@ -2815,7 +2815,7 @@
         <v>30</v>
       </c>
       <c r="H98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
@@ -2826,14 +2826,14 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B99" s="32">
         <f>1/(49000000)</f>
         <v>2.0408163265306123E-8</v>
       </c>
       <c r="C99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -2842,23 +2842,23 @@
         <v>12</v>
       </c>
       <c r="F99" t="s">
+        <v>78</v>
+      </c>
+      <c r="H99" t="s">
         <v>79</v>
-      </c>
-      <c r="H99" t="s">
-        <v>80</v>
       </c>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B100" s="32">
         <f>1/(49000000)</f>
         <v>2.0408163265306123E-8</v>
       </c>
       <c r="C100" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -2867,23 +2867,23 @@
         <v>12</v>
       </c>
       <c r="F100" t="s">
+        <v>81</v>
+      </c>
+      <c r="H100" t="s">
         <v>82</v>
-      </c>
-      <c r="H100" t="s">
-        <v>83</v>
       </c>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B101" s="32">
         <f>-0.41/1000</f>
         <v>-4.0999999999999999E-4</v>
       </c>
       <c r="C101" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D101" t="s">
         <v>13</v>
@@ -2892,23 +2892,23 @@
         <v>12</v>
       </c>
       <c r="F101" t="s">
+        <v>84</v>
+      </c>
+      <c r="H101" t="s">
         <v>85</v>
-      </c>
-      <c r="H101" t="s">
-        <v>86</v>
       </c>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B102">
         <f>-0.66/1000</f>
         <v>-6.6E-4</v>
       </c>
       <c r="C102" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D102" t="s">
         <v>13</v>
@@ -2917,23 +2917,23 @@
         <v>12</v>
       </c>
       <c r="F102" t="s">
+        <v>87</v>
+      </c>
+      <c r="H102" t="s">
         <v>88</v>
-      </c>
-      <c r="H102" t="s">
-        <v>89</v>
       </c>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B103">
         <f>-5.55/1000</f>
         <v>-5.5500000000000002E-3</v>
       </c>
       <c r="C103" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D103" t="s">
         <v>13</v>
@@ -2942,23 +2942,23 @@
         <v>12</v>
       </c>
       <c r="F103" t="s">
+        <v>90</v>
+      </c>
+      <c r="H103" t="s">
         <v>91</v>
-      </c>
-      <c r="H103" t="s">
-        <v>92</v>
       </c>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B104">
         <f>-0.1/1000</f>
         <v>-1E-4</v>
       </c>
       <c r="C104" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D104" t="s">
         <v>13</v>
@@ -2967,10 +2967,10 @@
         <v>12</v>
       </c>
       <c r="F104" t="s">
+        <v>93</v>
+      </c>
+      <c r="H104" t="s">
         <v>94</v>
-      </c>
-      <c r="H104" t="s">
-        <v>95</v>
       </c>
       <c r="I104"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>11</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="G116" s="13"/>
       <c r="H116" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -3188,19 +3188,19 @@
       </c>
       <c r="G117" s="13"/>
       <c r="H117" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B118" s="19">
         <f>1/(2500*80%*19.5)</f>
         <v>2.564102564102564E-5</v>
       </c>
       <c r="C118" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D118" t="s">
         <v>6</v>
@@ -3209,11 +3209,11 @@
         <v>12</v>
       </c>
       <c r="F118" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G118" s="13"/>
       <c r="H118" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -3221,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
@@ -3253,7 +3253,7 @@
         <v>11</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B128" s="19">
         <v>1</v>
@@ -3366,34 +3366,34 @@
     </row>
     <row r="129" spans="1:11">
       <c r="A129" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B129" s="19">
         <f>4.3*28.6</f>
         <v>122.98</v>
       </c>
       <c r="C129" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D129" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E129" t="s">
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B130" s="19">
         <v>1.34</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D130" t="s">
         <v>13</v>
@@ -3402,12 +3402,12 @@
         <v>12</v>
       </c>
       <c r="F130" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B131" s="19">
         <v>4.03</v>
@@ -3422,12 +3422,12 @@
         <v>12</v>
       </c>
       <c r="F131" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:11">
       <c r="A132" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B132" s="19">
         <v>8.34</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="133" spans="1:11">
       <c r="A133" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B133" s="19">
         <v>4.6399999999999997</v>
@@ -3459,7 +3459,7 @@
         <v>12</v>
       </c>
       <c r="F133" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
@@ -3499,7 +3499,7 @@
         <v>11</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C137" s="9"/>
       <c r="D137" s="9"/>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="143" spans="1:11">
       <c r="A143" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B143" s="19">
         <v>1</v>
@@ -3612,34 +3612,34 @@
     </row>
     <row r="144" spans="1:11">
       <c r="A144" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B144" s="19">
         <f>4.3*28.6</f>
         <v>122.98</v>
       </c>
       <c r="C144" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D144" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E144" t="s">
         <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="B145" s="19">
         <v>1.34</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D145" t="s">
         <v>13</v>
@@ -3648,12 +3648,12 @@
         <v>12</v>
       </c>
       <c r="F145" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B146" s="19">
         <v>4.03</v>
@@ -3668,12 +3668,12 @@
         <v>12</v>
       </c>
       <c r="F146" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B147" s="19">
         <v>4.6399999999999997</v>
@@ -3688,12 +3688,12 @@
         <v>12</v>
       </c>
       <c r="F147" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B148" s="19">
         <v>0.7</v>
@@ -3708,7 +3708,7 @@
         <v>12</v>
       </c>
       <c r="F148" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
storage electricity input from market for electricity, high voltage
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschlesinger\0.Joanna\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2D8C52-9E79-4761-9EB3-545791DA9922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8010D692-E6C7-4777-9D23-B812086CDBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B13" s="19">
         <f>1*1.12*1.15</f>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="81" spans="1:18" s="25" customFormat="1" ht="15.5">
       <c r="A81" s="41" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B81" s="44">
         <v>54</v>

</xml_diff>

<commit_message>
storage electricity input and output with high voltage instead of low voltage for all storage
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschlesinger\0.Joanna\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8010D692-E6C7-4777-9D23-B812086CDBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F246A64C-536E-4661-947F-243CB84EF852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
@@ -1140,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="18"/>
@@ -1164,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="20"/>
@@ -2500,7 +2500,7 @@
         <v>12</v>
       </c>
       <c r="G81" s="35" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H81" s="40" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
additionnal inventories modified to match with premise v.2.3.0dev1
</commit_message>
<xml_diff>
--- a/inventories/lci-FE2050.xlsx
+++ b/inventories/lci-FE2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschlesinger\0.Joanna\RTE_scenarios\inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AE05C8-1F16-496E-9C47-6E05FCAFEF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56835C8A-3E14-4A0D-AC41-90D0C97FE4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="133">
   <si>
     <t>Database</t>
   </si>
@@ -221,21 +221,9 @@
     <t>BoP, 20 years lifetime.</t>
   </si>
   <si>
-    <t>treatment of fuel cell stack, 1MWe, PEM</t>
-  </si>
-  <si>
-    <t>used fuel cell stack, 1MWe, PEM</t>
-  </si>
-  <si>
     <t>Stack EoL</t>
   </si>
   <si>
-    <t>treatment of fuel cell balance of plant, 1MWe, PEM</t>
-  </si>
-  <si>
-    <t>used fuel cell balance of plant, 1MWe, PEM</t>
-  </si>
-  <si>
     <t>BoP EoL</t>
   </si>
   <si>
@@ -347,9 +335,6 @@
     <t>geological hydrogen storage</t>
   </si>
   <si>
-    <t>WEU</t>
-  </si>
-  <si>
     <t>hydrogen storage</t>
   </si>
   <si>
@@ -441,6 +426,18 @@
   </si>
   <si>
     <t>coke production</t>
+  </si>
+  <si>
+    <t>treatment of electrolyzer stack, 1MWe, PEM</t>
+  </si>
+  <si>
+    <t>treatment of electrolyzer balance of plant, 1MWe, PEM</t>
+  </si>
+  <si>
+    <t>used electrolyzer stack, 1MWe, PEM</t>
+  </si>
+  <si>
+    <t>used electrolyzer balance of plant, 1MWe, PEM</t>
   </si>
 </sst>
 </file>
@@ -584,7 +581,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -644,6 +641,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Neutre" xfId="4" builtinId="28"/>
@@ -930,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A82" sqref="A76:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1148,7 +1147,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B13" s="19">
         <f>1*1.12*1.15</f>
@@ -1180,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="9"/>
@@ -1212,7 +1211,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1315,7 +1314,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B23" s="19">
         <v>1</v>
@@ -1339,7 +1338,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B24" s="19">
         <v>4.0404040404040398E-13</v>
@@ -1354,12 +1353,12 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B25" s="19">
         <v>7.5599999999999996E-6</v>
@@ -1374,12 +1373,12 @@
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B26" s="19">
         <v>-7.5599999999999996E-6</v>
@@ -1394,12 +1393,12 @@
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B27" s="19">
         <v>1.25125</v>
@@ -1419,7 +1418,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B28" s="19">
         <v>7.7000000000000001E-8</v>
@@ -1431,12 +1430,12 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B29" s="19">
         <v>1.4E-5</v>
@@ -1448,18 +1447,18 @@
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B30" s="19">
         <v>2.49876858810916E-4</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1470,24 +1469,24 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B31" s="19">
         <v>1.1580501231411899</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B32" s="19">
         <v>3.4499999999999999E-3</v>
@@ -1504,13 +1503,13 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B33" s="19">
         <v>2.3E-5</v>
       </c>
       <c r="D33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1521,13 +1520,13 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B34" s="19">
         <v>2.2999999999999999E-7</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -1538,13 +1537,13 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B35" s="19">
         <v>2.2770000000000001E-5</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1555,36 +1554,36 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B36" s="19">
         <v>0.15</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B37" s="19">
         <v>1.1583000000000001</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1598,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="9"/>
@@ -1630,7 +1629,7 @@
         <v>11</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -1733,7 +1732,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B47" s="19">
         <v>1</v>
@@ -1757,7 +1756,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B48" s="19">
         <v>1.3888999999999999E-11</v>
@@ -1772,7 +1771,7 @@
         <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G48" s="13"/>
       <c r="H48" s="18"/>
@@ -1780,7 +1779,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B49" s="19">
         <v>4.9730000000000003E-2</v>
@@ -1795,7 +1794,7 @@
         <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="18"/>
@@ -1803,19 +1802,19 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B50" s="19">
         <v>4.4479999999999899E-4</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="18"/>
@@ -1823,7 +1822,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B51" s="19">
         <v>1.5428571428571401E-4</v>
@@ -1835,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="18"/>
@@ -1843,7 +1842,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B52" s="19">
         <v>2.47445129042634E-4</v>
@@ -1872,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="9"/>
@@ -1904,7 +1903,7 @@
         <v>11</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -1920,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2007,7 +2006,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B62" s="19">
         <v>1</v>
@@ -2023,7 +2022,7 @@
         <v>18</v>
       </c>
       <c r="F62" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="18"/>
@@ -2031,7 +2030,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>1.0093999999999901</v>
@@ -2054,13 +2053,13 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B64">
         <v>1.0093999999999901</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -2069,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
@@ -2100,7 +2099,7 @@
     </row>
     <row r="66" spans="1:20">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B66">
         <v>9.3999999999998494E-3</v>
@@ -2130,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="35"/>
@@ -2311,8 +2310,8 @@
       <c r="T75" s="28"/>
     </row>
     <row r="76" spans="1:20" s="25" customFormat="1" ht="15.5">
-      <c r="A76" s="44" t="s">
-        <v>71</v>
+      <c r="A76" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="B76" s="44">
         <v>1</v>
@@ -2343,8 +2342,8 @@
       <c r="T76"/>
     </row>
     <row r="77" spans="1:20" s="25" customFormat="1" ht="15.5">
-      <c r="A77" s="44" t="s">
-        <v>69</v>
+      <c r="A77" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="B77" s="35">
         <f>(1/2963200)*4</f>
@@ -2378,8 +2377,8 @@
       <c r="R77"/>
     </row>
     <row r="78" spans="1:20" s="25" customFormat="1" ht="15.5">
-      <c r="A78" s="44" t="s">
-        <v>70</v>
+      <c r="A78" s="49" t="s">
+        <v>66</v>
       </c>
       <c r="B78" s="35">
         <f>1/2963200</f>
@@ -2413,8 +2412,8 @@
       <c r="R78"/>
     </row>
     <row r="79" spans="1:20" s="25" customFormat="1" ht="15.5">
-      <c r="A79" s="44" t="s">
-        <v>60</v>
+      <c r="A79" s="49" t="s">
+        <v>129</v>
       </c>
       <c r="B79" s="35">
         <f>B77*-1</f>
@@ -2431,10 +2430,10 @@
         <v>12</v>
       </c>
       <c r="G79" s="35" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="H79" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I79" s="35"/>
       <c r="J79"/>
@@ -2448,8 +2447,8 @@
       <c r="R79"/>
     </row>
     <row r="80" spans="1:20" s="25" customFormat="1" ht="15.5">
-      <c r="A80" s="44" t="s">
-        <v>63</v>
+      <c r="A80" s="49" t="s">
+        <v>130</v>
       </c>
       <c r="B80" s="35">
         <f>-1*B78</f>
@@ -2466,10 +2465,10 @@
         <v>12</v>
       </c>
       <c r="G80" s="35" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="H80" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I80" s="35"/>
       <c r="J80"/>
@@ -2483,8 +2482,8 @@
       <c r="R80"/>
     </row>
     <row r="81" spans="1:18" s="25" customFormat="1" ht="15.5">
-      <c r="A81" s="41" t="s">
-        <v>95</v>
+      <c r="A81" s="50" t="s">
+        <v>91</v>
       </c>
       <c r="B81" s="44">
         <v>54</v>
@@ -2503,7 +2502,7 @@
         <v>30</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I81" s="35"/>
       <c r="J81"/>
@@ -2517,7 +2516,7 @@
       <c r="R81"/>
     </row>
     <row r="82" spans="1:18" s="25" customFormat="1" ht="15.5">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B82" s="44">
@@ -2537,7 +2536,7 @@
         <v>23</v>
       </c>
       <c r="H82" s="35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I82" s="35"/>
       <c r="J82"/>
@@ -2582,7 +2581,7 @@
     </row>
     <row r="84" spans="1:18" s="25" customFormat="1" ht="15.5">
       <c r="A84" s="46" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B84" s="43">
         <f>(0.09*1000*20)/2963200</f>
@@ -2644,11 +2643,11 @@
         <v>1</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I87"/>
       <c r="M87" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:18">
@@ -2660,7 +2659,7 @@
       </c>
       <c r="I88"/>
       <c r="M88" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:18">
@@ -2668,7 +2667,7 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I89"/>
     </row>
@@ -2681,15 +2680,15 @@
       </c>
       <c r="I90"/>
       <c r="M90" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:18">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B91" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I91"/>
     </row>
@@ -2702,7 +2701,7 @@
       </c>
       <c r="I92"/>
       <c r="M92" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:18">
@@ -2710,11 +2709,11 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I93"/>
       <c r="M93" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:18">
@@ -2726,7 +2725,7 @@
       </c>
       <c r="I94"/>
       <c r="M94" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="15.5">
@@ -2736,7 +2735,7 @@
       <c r="B95"/>
       <c r="I95"/>
       <c r="M95" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="15.5">
@@ -2797,7 +2796,7 @@
     </row>
     <row r="98" spans="1:14">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B98">
         <v>1.33</v>
@@ -2815,7 +2814,7 @@
         <v>30</v>
       </c>
       <c r="H98" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
@@ -2826,7 +2825,7 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B99" s="32">
         <f>1/(49000000)</f>
@@ -2842,16 +2841,16 @@
         <v>12</v>
       </c>
       <c r="F99" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H99" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B100" s="32">
         <f>1/(49000000)</f>
@@ -2867,16 +2866,16 @@
         <v>12</v>
       </c>
       <c r="F100" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H100" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B101" s="32">
         <f>-0.41/1000</f>
@@ -2892,16 +2891,16 @@
         <v>12</v>
       </c>
       <c r="F101" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H101" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B102">
         <f>-0.66/1000</f>
@@ -2917,16 +2916,16 @@
         <v>12</v>
       </c>
       <c r="F102" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H102" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B103">
         <f>-5.55/1000</f>
@@ -2942,16 +2941,16 @@
         <v>12</v>
       </c>
       <c r="F103" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H103" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B104">
         <f>-0.1/1000</f>
@@ -2967,10 +2966,10 @@
         <v>12</v>
       </c>
       <c r="F104" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H104" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I104"/>
     </row>
@@ -3366,7 +3365,7 @@
     </row>
     <row r="129" spans="1:11">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B129" s="19">
         <f>4.3*28.6</f>
@@ -3387,7 +3386,7 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B130" s="19">
         <v>1.34</v>
@@ -3612,7 +3611,7 @@
     </row>
     <row r="144" spans="1:11">
       <c r="A144" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B144" s="19">
         <f>4.3*28.6</f>
@@ -3633,7 +3632,7 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B145" s="19">
         <v>1.34</v>

</xml_diff>